<commit_message>
Worked on multiple cheatsheets and added Node.js also
</commit_message>
<xml_diff>
--- a/Git and GitHub Cheatsheet.xlsx
+++ b/Git and GitHub Cheatsheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\conor\My Drive\Cheatsheet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\conor\My Drive\Cheatsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ADA26D1-AFD9-4C04-941B-1478C77351E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDA987B3-4D26-48D4-A724-2D3093E81591}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13740" yWindow="7740" windowWidth="15165" windowHeight="7845" xr2:uid="{CFA2EEE3-A297-4C77-8F4B-E4C68F45D0C6}"/>
+    <workbookView xWindow="-28920" yWindow="-885" windowWidth="29040" windowHeight="15720" xr2:uid="{CFA2EEE3-A297-4C77-8F4B-E4C68F45D0C6}"/>
   </bookViews>
   <sheets>
     <sheet name="Git Basic Commands" sheetId="1" r:id="rId1"/>
@@ -157,9 +157,6 @@
     <t>This command pulls the updates from GitHub and brings it down to the local branch. Pulls from the origin to the master branch</t>
   </si>
   <si>
-    <t>There may be times where you aren't able to push local work because the work on GitHub has been changed also. The solutoin to this is to pull first, sort out the errors, then push once again</t>
-  </si>
-  <si>
     <t>git branch -a</t>
   </si>
   <si>
@@ -182,13 +179,31 @@
   </si>
   <si>
     <t>Delete one of the git branches. Important to use a capital D</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">There may be times where you aren't able to push local work because the work on GitHub has been changed also. The solution to this is to pull first, sort out the errors, then push once again.
+If you really want to force through a change (could be risky if there's multiple people), do this command:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>git push -f origin main</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -198,6 +213,14 @@
     </font>
     <font>
       <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -276,9 +299,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -316,7 +339,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -422,7 +445,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -564,7 +587,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -575,7 +598,7 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -656,7 +679,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>18</v>
       </c>
@@ -667,7 +690,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" ht="105" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>19</v>
       </c>
@@ -675,7 +698,7 @@
         <v>23</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -688,34 +711,34 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>